<commit_message>
updating the work ratio, smarter dataframe and option for excel output
</commit_message>
<xml_diff>
--- a/src/excel/evogene-jira-analist/yearly-planning.xlsx
+++ b/src/excel/evogene-jira-analist/yearly-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\src\excel\evogene-jira-analist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06251E1-3589-4B17-B728-A232C08DB033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8906A2FB-88E1-4AEA-B949-30C559A7ACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -573,12 +573,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O10" sqref="O10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.58203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.9140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
adding the totals column to mission planning and changing the filename in work ratio
</commit_message>
<xml_diff>
--- a/src/excel/evogene-jira-analist/yearly-planning.xlsx
+++ b/src/excel/evogene-jira-analist/yearly-planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\utils\src\excel\evogene-jira-analist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8906A2FB-88E1-4AEA-B949-30C559A7ACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B39BE8-6606-4F4B-A6C0-981DB5462F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>Company Name</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Total Difference</t>
+  </si>
+  <si>
+    <t>Total Planned - Yearly</t>
+  </si>
+  <si>
+    <t>Total Time Spent - Yearly</t>
+  </si>
+  <si>
+    <t>Total Difference - Yearly</t>
   </si>
   <si>
     <t>AgPlenus</t>
@@ -571,23 +580,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O10" sqref="O10"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.9140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,13 +674,22 @@
       <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3">
         <v>2.54</v>
@@ -746,11 +763,20 @@
       <c r="Z2" s="5">
         <v>-13.33</v>
       </c>
+      <c r="AA2" s="3">
+        <v>30.5</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>31.12</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>-0.62</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C3" s="3">
         <v>2.08</v>
@@ -824,11 +850,20 @@
       <c r="Z3" s="5">
         <v>-20.98</v>
       </c>
+      <c r="AA3" s="3">
+        <v>25</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>35.56</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>-10.56</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3">
         <v>0.25</v>
@@ -902,13 +937,22 @@
       <c r="Z4" s="4">
         <v>1.75</v>
       </c>
+      <c r="AA4" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C5" s="3">
         <v>0.08</v>
@@ -982,11 +1026,20 @@
       <c r="Z5" s="4">
         <v>0.57999999999999996</v>
       </c>
+      <c r="AA5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -1060,11 +1113,20 @@
       <c r="Z6" s="4">
         <v>6.5</v>
       </c>
+      <c r="AA6" s="3">
+        <v>12</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AC6" s="4">
+        <v>11.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -1138,13 +1200,22 @@
       <c r="Z7" s="2">
         <v>0</v>
       </c>
+      <c r="AA7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -1218,11 +1289,20 @@
       <c r="Z8" s="2">
         <v>0</v>
       </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -1296,11 +1376,20 @@
       <c r="Z9" s="2">
         <v>0</v>
       </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -1374,13 +1463,22 @@
       <c r="Z10" s="2">
         <v>0</v>
       </c>
+      <c r="AA10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3">
         <v>1.25</v>
@@ -1454,11 +1552,20 @@
       <c r="Z11" s="5">
         <v>-3</v>
       </c>
+      <c r="AA11" s="3">
+        <v>15</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>11.75</v>
+      </c>
+      <c r="AC11" s="4">
+        <v>3.25</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3">
         <v>20</v>
@@ -1532,11 +1639,20 @@
       <c r="Z12" s="4">
         <v>124.75</v>
       </c>
+      <c r="AA12" s="3">
+        <v>240</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>15.25</v>
+      </c>
+      <c r="AC12" s="4">
+        <v>224.75</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -1610,13 +1726,22 @@
       <c r="Z13" s="5">
         <v>-1.62</v>
       </c>
+      <c r="AA13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="AC13" s="5">
+        <v>-1.62</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3">
         <v>6.8</v>
@@ -1690,11 +1815,20 @@
       <c r="Z14" s="4">
         <v>6.98</v>
       </c>
+      <c r="AA14" s="3">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>40.619999999999997</v>
+      </c>
+      <c r="AC14" s="4">
+        <v>40.97</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3">
         <v>20.58</v>
@@ -1768,11 +1902,20 @@
       <c r="Z15" s="5">
         <v>-149.86000000000001</v>
       </c>
+      <c r="AA15" s="3">
+        <v>247</v>
+      </c>
+      <c r="AB15" s="2">
+        <v>293.95</v>
+      </c>
+      <c r="AC15" s="5">
+        <v>-46.95</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3">
         <v>19.75</v>
@@ -1846,13 +1989,22 @@
       <c r="Z16" s="5">
         <v>-54.5</v>
       </c>
+      <c r="AA16" s="3">
+        <v>237</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>192.75</v>
+      </c>
+      <c r="AC16" s="4">
+        <v>44.25</v>
+      </c>
     </row>
-    <row r="17" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -1926,11 +2078,20 @@
       <c r="Z17" s="2">
         <v>0</v>
       </c>
+      <c r="AA17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3">
         <v>2</v>
@@ -2004,11 +2165,20 @@
       <c r="Z18" s="4">
         <v>14</v>
       </c>
+      <c r="AA18" s="3">
+        <v>24</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="19" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -2082,13 +2252,22 @@
       <c r="Z19" s="2">
         <v>0</v>
       </c>
+      <c r="AA19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -2162,11 +2341,20 @@
       <c r="Z20" s="2">
         <v>0</v>
       </c>
+      <c r="AA20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -2240,11 +2428,20 @@
       <c r="Z21" s="2">
         <v>0</v>
       </c>
+      <c r="AA21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -2318,13 +2515,22 @@
       <c r="Z22" s="2">
         <v>0</v>
       </c>
+      <c r="AA22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3">
         <v>23.3</v>
@@ -2398,11 +2604,20 @@
       <c r="Z23" s="5">
         <v>-30.23</v>
       </c>
+      <c r="AA23" s="3">
+        <v>279.60000000000002</v>
+      </c>
+      <c r="AB23" s="2">
+        <v>193.33</v>
+      </c>
+      <c r="AC23" s="4">
+        <v>86.27</v>
+      </c>
     </row>
-    <row r="24" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3">
         <v>3.08</v>
@@ -2476,11 +2691,20 @@
       <c r="Z24" s="4">
         <v>17.21</v>
       </c>
+      <c r="AA24" s="3">
+        <v>37</v>
+      </c>
+      <c r="AB24" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="AC24" s="4">
+        <v>32.619999999999997</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3">
         <v>14.3</v>
@@ -2554,13 +2778,22 @@
       <c r="Z25" s="5">
         <v>-6.28</v>
       </c>
+      <c r="AA25" s="3">
+        <v>171.6</v>
+      </c>
+      <c r="AB25" s="2">
+        <v>106.38</v>
+      </c>
+      <c r="AC25" s="4">
+        <v>65.22</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C26" s="3">
         <v>3.25</v>
@@ -2634,11 +2867,20 @@
       <c r="Z26" s="5">
         <v>-16.25</v>
       </c>
+      <c r="AA26" s="3">
+        <v>39</v>
+      </c>
+      <c r="AB26" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC26" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C27" s="3">
         <v>1.97</v>
@@ -2712,11 +2954,20 @@
       <c r="Z27" s="5">
         <v>-9.85</v>
       </c>
+      <c r="AA27" s="3">
+        <v>23.64</v>
+      </c>
+      <c r="AB27" s="2">
+        <v>23.64</v>
+      </c>
+      <c r="AC27" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C28" s="3">
         <v>1.64</v>
@@ -2790,13 +3041,22 @@
       <c r="Z28" s="5">
         <v>-8.2100000000000009</v>
       </c>
+      <c r="AA28" s="3">
+        <v>19.68</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>19.690000000000001</v>
+      </c>
+      <c r="AC28" s="5">
+        <v>-0.01</v>
+      </c>
     </row>
-    <row r="29" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -2870,11 +3130,20 @@
       <c r="Z29" s="5">
         <v>-8</v>
       </c>
+      <c r="AA29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>8</v>
+      </c>
+      <c r="AC29" s="5">
+        <v>-8</v>
+      </c>
     </row>
-    <row r="30" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3">
         <v>16.829999999999998</v>
@@ -2948,11 +3217,20 @@
       <c r="Z30" s="4">
         <v>78.27</v>
       </c>
+      <c r="AA30" s="3">
+        <v>202</v>
+      </c>
+      <c r="AB30" s="2">
+        <v>39.56</v>
+      </c>
+      <c r="AC30" s="4">
+        <v>162.44</v>
+      </c>
     </row>
-    <row r="31" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -3026,13 +3304,22 @@
       <c r="Z31" s="5">
         <v>-0.56000000000000005</v>
       </c>
+      <c r="AA31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="AC31" s="5">
+        <v>-0.56000000000000005</v>
+      </c>
     </row>
-    <row r="32" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C32" s="3">
         <v>5.15</v>
@@ -3106,11 +3393,20 @@
       <c r="Z32" s="4">
         <v>10.92</v>
       </c>
+      <c r="AA32" s="3">
+        <v>61.8</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>25.12</v>
+      </c>
+      <c r="AC32" s="4">
+        <v>36.67</v>
+      </c>
     </row>
-    <row r="33" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C33" s="3">
         <v>20.170000000000002</v>
@@ -3184,11 +3480,20 @@
       <c r="Z33" s="4">
         <v>21.25</v>
       </c>
+      <c r="AA33" s="3">
+        <v>242</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>119.91</v>
+      </c>
+      <c r="AC33" s="4">
+        <v>122.09</v>
+      </c>
     </row>
-    <row r="34" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C34" s="3">
         <v>16.75</v>
@@ -3262,13 +3567,22 @@
       <c r="Z34" s="4">
         <v>24.88</v>
       </c>
+      <c r="AA34" s="3">
+        <v>201</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>92.38</v>
+      </c>
+      <c r="AC34" s="4">
+        <v>108.62</v>
+      </c>
     </row>
-    <row r="35" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C35" s="3">
         <v>0</v>
@@ -3342,11 +3656,20 @@
       <c r="Z35" s="5">
         <v>-2.25</v>
       </c>
+      <c r="AA35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="AC35" s="5">
+        <v>-2.25</v>
+      </c>
     </row>
-    <row r="36" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
@@ -3420,11 +3743,20 @@
       <c r="Z36" s="5">
         <v>-18.809999999999999</v>
       </c>
+      <c r="AA36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="AC36" s="5">
+        <v>-18.809999999999999</v>
+      </c>
     </row>
-    <row r="37" spans="1:26" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
@@ -3496,6 +3828,15 @@
         <v>1.5</v>
       </c>
       <c r="Z37" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="AA37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="AC37" s="5">
         <v>-1.5</v>
       </c>
     </row>

</xml_diff>